<commit_message>
Add create and edit ticket api
</commit_message>
<xml_diff>
--- a/notes/Data Dictionary.xlsx
+++ b/notes/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\Career\Projects\katol-bugtracker\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46617DAB-DF06-4DDE-ABAE-188685596073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD22111-C194-475B-91A4-420D71C6DF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7716" yWindow="1728" windowWidth="17280" windowHeight="8964" xr2:uid="{ECFFB2B3-C9A8-488D-9308-DD302F669E05}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECFFB2B3-C9A8-488D-9308-DD302F669E05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>User</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Ticket</t>
   </si>
   <si>
-    <t>Comments [ { name, date, content }]</t>
-  </si>
-  <si>
     <t>Date Last updated</t>
   </si>
   <si>
@@ -150,10 +147,19 @@
     <t>Status - "Open, Cancelled, Resolved"</t>
   </si>
   <si>
-    <t>Log - [{User, Date, Action} ]</t>
-  </si>
-  <si>
     <t>Options { notifications: boolean }</t>
+  </si>
+  <si>
+    <t>Comments [ { author_id, author, name, date, content }]</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -623,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD96939C-3D71-4DA1-93EE-2D7713BC35D2}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,11 +657,11 @@
       </c>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="3"/>
       <c r="K3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" s="14"/>
     </row>
@@ -669,7 +675,7 @@
       </c>
       <c r="F4" s="5"/>
       <c r="H4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="5"/>
       <c r="K4" s="4" t="s">
@@ -683,15 +689,15 @@
       </c>
       <c r="C5" s="5"/>
       <c r="E5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5"/>
       <c r="H5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="5"/>
       <c r="K5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L5" s="5"/>
     </row>
@@ -701,17 +707,17 @@
       </c>
       <c r="C6" s="5"/>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="5"/>
       <c r="H6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="K6" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="10"/>
+      <c r="K6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
@@ -719,13 +725,17 @@
       </c>
       <c r="C7" s="5"/>
       <c r="E7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="5"/>
       <c r="H7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="10"/>
+      <c r="K7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
@@ -736,10 +746,10 @@
         <v>13</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="K8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="3"/>
+      <c r="K8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
@@ -747,13 +757,9 @@
       </c>
       <c r="C9" s="5"/>
       <c r="H9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="K9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
@@ -768,10 +774,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="K10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5"/>
+      <c r="K10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
@@ -783,27 +789,27 @@
       </c>
       <c r="F11" s="5"/>
       <c r="H11" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" s="10"/>
       <c r="K11" s="6" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="K12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="10"/>
+      <c r="K12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
@@ -811,9 +817,13 @@
       </c>
       <c r="C13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="5"/>
+      <c r="K13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
@@ -822,43 +832,47 @@
       <c r="C14" s="8"/>
       <c r="D14" s="1"/>
       <c r="E14" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="5"/>
+      <c r="K14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E15" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E16" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E17" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E18" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E19" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E20" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="10"/>
     </row>

</xml_diff>